<commit_message>
fix bugs in deploying the system
</commit_message>
<xml_diff>
--- a/vnpy_self/strategy1_schedule.xlsx
+++ b/vnpy_self/strategy1_schedule.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
   <si>
     <t>date</t>
   </si>
@@ -32,34 +32,31 @@
     <t>2023-03-13</t>
   </si>
   <si>
-    <t>IH2303,IH2306</t>
+    <t>IH2306.CFFEX,IH2309.CFFEX</t>
   </si>
   <si>
     <t>2023-06-12</t>
   </si>
   <si>
-    <t>IH2306,IH2309</t>
+    <t>IH2309.CFFEX,IH2312.CFFEX</t>
   </si>
   <si>
     <t>2023-09-11</t>
   </si>
   <si>
-    <t>IH2309,IH2312</t>
+    <t>IH2312.CFFEX,IH2403.CFFEX</t>
   </si>
   <si>
     <t>2023-12-11</t>
   </si>
   <si>
-    <t>IH2312,IH2403</t>
+    <t>IH2403.CFFEX,IH2406.CFFEX</t>
   </si>
   <si>
     <t>2024-03-11</t>
   </si>
   <si>
-    <t>IH2403,IH2406</t>
-  </si>
-  <si>
-    <t/>
+    <t>IH2406.CFFEX,IH2409.CFFEX</t>
   </si>
 </sst>
 </file>
@@ -67,7 +64,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -77,13 +74,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -123,7 +114,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="5">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -132,15 +123,6 @@
       <alignment horizontal="general"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -454,20 +436,20 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="3" width="32.29071428571429" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -475,7 +457,7 @@
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -483,7 +465,7 @@
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B4" s="2" t="s">
@@ -491,7 +473,7 @@
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B5" s="2" t="s">
@@ -499,7 +481,7 @@
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B6" s="2" t="s">
@@ -507,12 +489,8 @@
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
-      <c r="A7" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>14</v>
-      </c>
+      <c r="A7" s="1"/>
+      <c r="B7" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>